<commit_message>
refactored and commented code
</commit_message>
<xml_diff>
--- a/docs/describe_output_structure.xlsx
+++ b/docs/describe_output_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shank\Google Drive\Jupyter Data\Consulting\External\Kering\Sourcev1\Coding\dbt_eda_tools\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2329582D-D6E1-4797-922C-97BD8B5E342D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEC87A8-3FE8-41C8-9E99-E9C25121CBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="240" windowWidth="25995" windowHeight="14460" xr2:uid="{D8851B85-212C-449E-96F6-3CD373D9F75E}"/>
+    <workbookView xWindow="23130" yWindow="1785" windowWidth="21600" windowHeight="11295" xr2:uid="{D8851B85-212C-449E-96F6-3CD373D9F75E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t># of rows</t>
   </si>
   <si>
-    <t>Dataset</t>
-  </si>
-  <si>
     <t># of Text columns</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>Detail</t>
-  </si>
-  <si>
-    <t>Column</t>
   </si>
   <si>
     <t>{
@@ -131,6 +125,12 @@
   </si>
   <si>
     <t># of Boolean Columns</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>column</t>
   </si>
 </sst>
 </file>
@@ -529,138 +529,138 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="31.5703125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="156" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>